<commit_message>
D O N E   B O I Z Z Z
</commit_message>
<xml_diff>
--- a/StockMarket.AdminService/UploadFiles/sample_stock_data.xlsx
+++ b/StockMarket.AdminService/UploadFiles/sample_stock_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Company Code</t>
   </si>
@@ -29,12 +29,6 @@
     <t>Stock Exchange</t>
   </si>
   <si>
-    <t>BSE</t>
-  </si>
-  <si>
-    <t>500112 </t>
-  </si>
-  <si>
     <t>Price Per Share(in Rs)</t>
   </si>
   <si>
@@ -69,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">  11:10:00</t>
+  </si>
+  <si>
+    <t>NSE</t>
   </si>
 </sst>
 </file>
@@ -414,7 +411,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,21 +430,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>356.23</v>
@@ -456,15 +453,15 @@
         <v>43624</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>361.31</v>
@@ -473,15 +470,15 @@
         <v>43624</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>358.12</v>
@@ -490,15 +487,15 @@
         <v>43624</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5">
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>357.09</v>
@@ -507,15 +504,15 @@
         <v>43624</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>353.62</v>
@@ -524,15 +521,15 @@
         <v>43624</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="A7">
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>349.56</v>
@@ -541,15 +538,15 @@
         <v>43624</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
+      <c r="A8">
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>351.43</v>
@@ -558,15 +555,15 @@
         <v>43624</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>350.12</v>
@@ -575,15 +572,15 @@
         <v>43624</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
+      <c r="A10">
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>348.91</v>
@@ -592,7 +589,7 @@
         <v>43624</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" ht="26.45" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>